<commit_message>
working branch with argparse, json/xml transform, single-file transform
</commit_message>
<xml_diff>
--- a/nida_datashare/study_metadata.xlsx
+++ b/nida_datashare/study_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcheadle\projects\heal_metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcheadle\projects\HEALmunger\nida_datashare\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5F800F5-CCF0-421A-95C9-090D3912A54F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CCD403D-FB8A-40AC-B6F9-142F91D64423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1299,6 +1299,7 @@
     <filterColumn colId="5">
       <filters>
         <filter val="Yes"/>
+        <filter val="Yes - needs cleaning"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1581,7 +1582,7 @@
   <dimension ref="A1:G77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1642,7 +1643,7 @@
         <v>43875</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1665,7 +1666,7 @@
         <v>42878</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>42878</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1711,7 +1712,7 @@
         <v>42878</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>42878</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -1803,7 +1804,7 @@
         <v>43985</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>50</v>
       </c>
@@ -1826,7 +1827,7 @@
         <v>41977</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>55</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>42249</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>60</v>
       </c>
@@ -1872,7 +1873,7 @@
         <v>41977</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>65</v>
       </c>
@@ -1895,7 +1896,7 @@
         <v>41977</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>69</v>
       </c>
@@ -2010,7 +2011,7 @@
         <v>43227</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>93</v>
       </c>
@@ -2033,7 +2034,7 @@
         <v>42249</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>98</v>
       </c>
@@ -2260,7 +2261,7 @@
         <v>39419</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>120</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>152</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G30" s="5">
         <v>40024</v>
@@ -2530,7 +2531,7 @@
         <v>39659</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>205</v>
       </c>
@@ -2599,7 +2600,7 @@
         <v>40162</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>208</v>
       </c>
@@ -2622,7 +2623,7 @@
         <v>40716</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>210</v>
       </c>
@@ -2642,7 +2643,7 @@
         <v>41873</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>209</v>
       </c>
@@ -2708,7 +2709,7 @@
         <v>40849</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>213</v>
       </c>
@@ -2731,7 +2732,7 @@
         <v>41823</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>214</v>
       </c>
@@ -2754,7 +2755,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>253</v>
       </c>
@@ -2800,7 +2801,7 @@
         <v>41597</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>255</v>
       </c>
@@ -2823,7 +2824,7 @@
         <v>41884</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>256</v>
       </c>
@@ -2846,7 +2847,7 @@
         <v>42118</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>257</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>43350</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>258</v>
       </c>
@@ -2892,7 +2893,7 @@
         <v>43112</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>259</v>
       </c>
@@ -2915,7 +2916,7 @@
         <v>41773</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>260</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>43294</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>261</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>44113</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>262</v>
       </c>
@@ -2984,7 +2985,7 @@
         <v>42992</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>303</v>
       </c>
@@ -3007,7 +3008,7 @@
         <v>42992</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>304</v>
       </c>
@@ -3030,7 +3031,7 @@
         <v>41977</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>305</v>
       </c>
@@ -3053,7 +3054,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>306</v>
       </c>
@@ -3076,7 +3077,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>307</v>
       </c>
@@ -3099,7 +3100,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>308</v>
       </c>
@@ -3122,7 +3123,7 @@
         <v>42583</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>309</v>
       </c>
@@ -3237,7 +3238,7 @@
         <v>43480</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>353</v>
       </c>
@@ -3306,7 +3307,7 @@
         <v>43090</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>356</v>
       </c>
@@ -3329,7 +3330,7 @@
         <v>42249</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>357</v>
       </c>

</xml_diff>